<commit_message>
Ajout temporisation dans la generation scenario
</commit_message>
<xml_diff>
--- a/UnitTest 00.xlsx
+++ b/UnitTest 00.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>Target</t>
   </si>
@@ -25,9 +25,6 @@
     <t>STEP 1</t>
   </si>
   <si>
-    <t>TEMPO</t>
-  </si>
-  <si>
     <t>Action</t>
   </si>
   <si>
@@ -128,6 +125,18 @@
   </si>
   <si>
     <t>Test 1.2</t>
+  </si>
+  <si>
+    <t>4000</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>7000</t>
+  </si>
+  <si>
+    <t>DELAY</t>
   </si>
 </sst>
 </file>
@@ -205,10 +214,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -216,6 +225,9 @@
   <dxfs count="9">
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="1" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -230,9 +242,6 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="1" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <color theme="0"/>
@@ -245,12 +254,12 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <border>
-        <top/>
-      </border>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCE6F1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border>
@@ -261,14 +270,6 @@
       <border>
         <top/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCE6F1"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -288,14 +289,22 @@
         <horizontal/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <border>
+        <top/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Description table" pivot="0" count="5">
-      <tableStyleElement type="totalRow" dxfId="4"/>
-      <tableStyleElement type="firstColumn" dxfId="8"/>
+      <tableStyleElement type="totalRow" dxfId="8"/>
+      <tableStyleElement type="firstColumn" dxfId="7"/>
       <tableStyleElement type="firstRowStripe" dxfId="6"/>
       <tableStyleElement type="secondRowStripe" dxfId="5"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="7"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="4"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -308,21 +317,21 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table_Action_1.2" displayName="Table_Action_1.2" ref="B5:Q13" totalsRowCount="1">
-  <autoFilter ref="B5:Q6"/>
+  <autoFilter ref="B5:Q12"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="Target" totalsRowLabel="TEMPO" dataDxfId="3" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Target" totalsRowLabel="DELAY" dataDxfId="3" totalsRowDxfId="0"/>
     <tableColumn id="2" name="Location"/>
     <tableColumn id="3" name="STEP 1"/>
-    <tableColumn id="4" name="STEP 2"/>
+    <tableColumn id="4" name="STEP 2" totalsRowLabel="4000"/>
     <tableColumn id="5" name="STEP 3"/>
     <tableColumn id="6" name="STEP 4"/>
     <tableColumn id="7" name="STEP 5"/>
-    <tableColumn id="8" name="STEP 6"/>
+    <tableColumn id="8" name="STEP 6" totalsRowLabel="5000"/>
     <tableColumn id="9" name="STEP 7"/>
     <tableColumn id="10" name="STEP 8"/>
     <tableColumn id="11" name="STEP 9"/>
     <tableColumn id="12" name="STEP 10"/>
-    <tableColumn id="13" name="STEP 11"/>
+    <tableColumn id="13" name="STEP 11" totalsRowLabel="7000"/>
     <tableColumn id="14" name="STEP 12"/>
     <tableColumn id="15" name="STEP 13"/>
     <tableColumn id="16" name="STEP 14"/>
@@ -334,9 +343,9 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table_Check_1.2" displayName="Table_Check_1.2" ref="B15:Q15" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="16">
-    <tableColumn id="1" name="Target" dataDxfId="1"/>
+    <tableColumn id="1" name="Target" dataDxfId="2"/>
     <tableColumn id="2" name="Location"/>
-    <tableColumn id="3" name="STEP 1" headerRowDxfId="2"/>
+    <tableColumn id="3" name="STEP 1" headerRowDxfId="1"/>
     <tableColumn id="4" name="Colonne1"/>
     <tableColumn id="5" name="Colonne2"/>
     <tableColumn id="6" name="Colonne3"/>
@@ -671,7 +680,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,70 +691,70 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
         <v>29</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s">
         <v>30</v>
       </c>
-      <c r="F3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
         <v>31</v>
       </c>
-      <c r="H3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" t="s">
         <v>32</v>
       </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" t="s">
         <v>33</v>
       </c>
-      <c r="L3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" t="s">
         <v>34</v>
       </c>
-      <c r="N3" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" t="s">
         <v>35</v>
       </c>
-      <c r="P3" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C4" s="6"/>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
+      <c r="A5" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -757,70 +766,70 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>16</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>17</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>18</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>19</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>20</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>21</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>22</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>23</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>24</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>25</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>26</v>
       </c>
-      <c r="Q5" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="A6" s="6"/>
       <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -834,10 +843,10 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -851,10 +860,10 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -868,10 +877,10 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -885,10 +894,10 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -899,10 +908,10 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -916,18 +925,27 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>3</v>
+        <v>40</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" t="s">
+        <v>38</v>
+      </c>
+      <c r="N13" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>5</v>
+      <c r="A15" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15">
         <v>0</v>

</xml_diff>